<commit_message>
adding classifier test notebook
</commit_message>
<xml_diff>
--- a/l1t_data/trigger_rates.xlsx
+++ b/l1t_data/trigger_rates.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wilkie/Library/CloudStorage/Box-Box/Threadwork/Simulations/Papers/HEP Detectors/CMS/L1T data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wilkie/code/system_flow/l1t_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FA09161-6D21-684A-B923-790E201C15D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B3F84A0-9861-6647-9729-37317AB59C3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="27500" yWindow="2280" windowWidth="19760" windowHeight="20680" xr2:uid="{BF612227-1505-0B45-96FC-314275F0E0E2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Muon</t>
   </si>
@@ -78,18 +78,36 @@
   </si>
   <si>
     <t>Tau proportions</t>
+  </si>
+  <si>
+    <t>Jet Threshold</t>
+  </si>
+  <si>
+    <t>Muon Threshold</t>
+  </si>
+  <si>
+    <t>Egamma Threshold</t>
+  </si>
+  <si>
+    <t>Tau Threshold</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -113,8 +131,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -449,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47220944-6CAF-6A45-AB44-4DB26F76941D}">
-  <dimension ref="A1:N13"/>
+  <dimension ref="A1:R13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1:R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -460,7 +479,7 @@
     <col min="1" max="1" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -503,8 +522,20 @@
       <c r="N1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -525,19 +556,19 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <f>C2*$B2</f>
+        <f t="shared" ref="G2:G13" si="0">C2*$B2</f>
         <v>0.01</v>
       </c>
       <c r="H2">
-        <f>D2*$B2</f>
+        <f t="shared" ref="H2:H13" si="1">D2*$B2</f>
         <v>0</v>
       </c>
       <c r="I2">
-        <f>E2*$B2</f>
+        <f t="shared" ref="I2:I13" si="2">E2*$B2</f>
         <v>0</v>
       </c>
       <c r="J2">
-        <f>F2*$B2</f>
+        <f t="shared" ref="J2:J13" si="3">F2*$B2</f>
         <v>0</v>
       </c>
       <c r="K2">
@@ -556,13 +587,25 @@
         <f>SUM(J2:J13)</f>
         <v>0.18</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O2" s="1">
+        <v>320</v>
+      </c>
+      <c r="P2" s="1">
+        <v>22</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>30</v>
+      </c>
+      <c r="R2" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2.6</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B13" si="0">A3/100</f>
+        <f t="shared" ref="B3:B13" si="4">A3/100</f>
         <v>2.6000000000000002E-2</v>
       </c>
       <c r="C3">
@@ -578,389 +621,389 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <f>C3*$B3</f>
+        <f t="shared" si="0"/>
         <v>2.6000000000000002E-2</v>
       </c>
       <c r="H3">
-        <f>D3*$B3</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I3">
-        <f>E3*$B3</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J3">
-        <f>F3*$B3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3.2</v>
       </c>
       <c r="B4">
+        <f t="shared" si="4"/>
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
         <f t="shared" si="0"/>
         <v>3.2000000000000001E-2</v>
       </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <f>C4*$B4</f>
+      <c r="H4">
+        <f t="shared" si="1"/>
         <v>3.2000000000000001E-2</v>
       </c>
-      <c r="H4">
-        <f>D4*$B4</f>
-        <v>3.2000000000000001E-2</v>
-      </c>
       <c r="I4">
-        <f>E4*$B4</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J4">
-        <f>F4*$B4</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3.3</v>
       </c>
       <c r="B5">
+        <f t="shared" si="4"/>
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="1"/>
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <f>C5*$B5</f>
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <f>D5*$B5</f>
+      <c r="I5">
+        <f t="shared" si="2"/>
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="I5">
-        <f>E5*$B5</f>
-        <v>3.3000000000000002E-2</v>
-      </c>
       <c r="J5">
-        <f>F5*$B5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4.5999999999999996</v>
       </c>
       <c r="B6">
+        <f t="shared" si="4"/>
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
         <f t="shared" si="0"/>
         <v>4.5999999999999999E-2</v>
       </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <f>C6*$B6</f>
+      <c r="H6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="2"/>
         <v>4.5999999999999999E-2</v>
       </c>
-      <c r="H6">
-        <f>D6*$B6</f>
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <f>E6*$B6</f>
-        <v>4.5999999999999999E-2</v>
-      </c>
       <c r="J6">
-        <f>F6*$B6</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5.3</v>
       </c>
       <c r="B7">
+        <f t="shared" si="4"/>
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
         <f t="shared" si="0"/>
         <v>5.2999999999999999E-2</v>
       </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7">
-        <f>C7*$B7</f>
+      <c r="H7">
+        <f t="shared" si="1"/>
         <v>5.2999999999999999E-2</v>
       </c>
-      <c r="H7">
-        <f>D7*$B7</f>
+      <c r="I7">
+        <f t="shared" si="2"/>
         <v>5.2999999999999999E-2</v>
       </c>
-      <c r="I7">
-        <f>E7*$B7</f>
+      <c r="J7">
+        <f t="shared" si="3"/>
         <v>5.2999999999999999E-2</v>
       </c>
-      <c r="J7">
-        <f>F7*$B7</f>
-        <v>5.2999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6.4</v>
       </c>
       <c r="B8">
+        <f t="shared" si="4"/>
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="2"/>
         <v>6.4000000000000001E-2</v>
       </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <f>C8*$B8</f>
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <f>D8*$B8</f>
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <f>E8*$B8</f>
-        <v>6.4000000000000001E-2</v>
-      </c>
       <c r="J8">
-        <f>F8*$B8</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>9.8000000000000007</v>
       </c>
       <c r="B9">
+        <f t="shared" si="4"/>
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="1"/>
         <v>9.8000000000000004E-2</v>
       </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <f>C9*$B9</f>
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <f>D9*$B9</f>
-        <v>9.8000000000000004E-2</v>
-      </c>
       <c r="I9">
-        <f>E9*$B9</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J9">
-        <f>F9*$B9</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>11.5</v>
       </c>
       <c r="B10">
+        <f t="shared" si="4"/>
+        <v>0.115</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
         <f t="shared" si="0"/>
         <v>0.115</v>
       </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <f>C10*$B10</f>
-        <v>0.115</v>
-      </c>
       <c r="H10">
-        <f>D10*$B10</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I10">
-        <f>E10*$B10</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J10">
-        <f>F10*$B10</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>12.7</v>
       </c>
       <c r="B11">
+        <f t="shared" si="4"/>
+        <v>0.127</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="3"/>
         <v>0.127</v>
       </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <v>1</v>
-      </c>
-      <c r="G11">
-        <f>C11*$B11</f>
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <f>D11*$B11</f>
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <f>E11*$B11</f>
-        <v>0</v>
-      </c>
-      <c r="J11">
-        <f>F11*$B11</f>
-        <v>0.127</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>14.8</v>
       </c>
       <c r="B12">
+        <f t="shared" si="4"/>
+        <v>0.14800000000000002</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="1"/>
         <v>0.14800000000000002</v>
       </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-      <c r="G12">
-        <f>C12*$B12</f>
-        <v>0</v>
-      </c>
-      <c r="H12">
-        <f>D12*$B12</f>
-        <v>0.14800000000000002</v>
-      </c>
       <c r="I12">
-        <f>E12*$B12</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J12">
-        <f>F12*$B12</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>24.8</v>
       </c>
       <c r="B13">
+        <f t="shared" si="4"/>
+        <v>0.248</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="2"/>
         <v>0.248</v>
       </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="G13">
-        <f>C13*$B13</f>
-        <v>0</v>
-      </c>
-      <c r="H13">
-        <f>D13*$B13</f>
-        <v>0</v>
-      </c>
-      <c r="I13">
-        <f>E13*$B13</f>
-        <v>0.248</v>
-      </c>
       <c r="J13">
-        <f>F13*$B13</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>